<commit_message>
Adición de tabla de servicios de cortinas
</commit_message>
<xml_diff>
--- a/tabla de servicios_Universal.xlsx
+++ b/tabla de servicios_Universal.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio\Documents\Facultad Ciencias Fisicas y Matematicas\Ramos\10º Semestre\Introducción al Taller de Diseño\Proyecto\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="23580" windowHeight="10110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ID_01" sheetId="3" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
   <si>
     <t>Descripcion</t>
   </si>
@@ -105,9 +110,6 @@
     <t>Control</t>
   </si>
   <si>
-    <t>3.101 - 3.303 - 3.304 - 3.305</t>
-  </si>
-  <si>
     <t>1.102 - 3.301 - 3.302</t>
   </si>
   <si>
@@ -127,12 +129,55 @@
   </si>
   <si>
     <t>Cortinas : 03</t>
+  </si>
+  <si>
+    <t>Sensor de luminosidad exterior</t>
+  </si>
+  <si>
+    <t>Sensor de temperatura</t>
+  </si>
+  <si>
+    <t>float [-55, 150]</t>
+  </si>
+  <si>
+    <t>Nivel de Iluminación exterior</t>
+  </si>
+  <si>
+    <t>Temperatura interior (ºC)</t>
+  </si>
+  <si>
+    <t>Programación de cortinas definida por el usuario (tiempo)</t>
+  </si>
+  <si>
+    <t>Estado de cortinas en cada habitación según programación temporal del usuario</t>
+  </si>
+  <si>
+    <t>Variable de "override" de control por nivel de temperatura</t>
+  </si>
+  <si>
+    <t>ON/OFF de relé para control de cortinas</t>
+  </si>
+  <si>
+    <t>Activación de control manual de cortinas 
+[switch en cada habitación]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.101 - 3.303 - 3.304 - 3.305 - 3.306 - 3.307 - 3.308 </t>
+  </si>
+  <si>
+    <t>Nivel mínimo/máximo de luz interior requerido para mover cortinas</t>
+  </si>
+  <si>
+    <t>Nivel mínimo/máximo de luz exterior requerido para mover cortinas</t>
+  </si>
+  <si>
+    <t>Nivel mínimo/máximo de temperatura requerido para mover cortinas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -349,7 +394,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -400,28 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -433,6 +457,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="7" borderId="2" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -442,49 +520,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -502,6 +556,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -550,7 +607,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -583,9 +640,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -618,6 +692,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -793,25 +884,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>33</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>24</v>
@@ -832,11 +923,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="43" t="s">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="38" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="9">
@@ -851,51 +942,51 @@
       </c>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="44"/>
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="4">
         <v>102</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="4">
-        <v>1.101</v>
+      <c r="E3" s="35">
+        <v>1101</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="21"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="21"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="21"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="21"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="21"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="21"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="21"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
     </row>
   </sheetData>
@@ -908,24 +999,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="7" max="30" width="11.42578125" style="10"/>
+    <col min="4" max="4" width="23.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="7" max="30" width="11.44140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>24</v>
@@ -946,11 +1039,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="1:30" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="45" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="3">
@@ -988,9 +1081,9 @@
       <c r="AC2" s="10"/>
       <c r="AD2" s="10"/>
     </row>
-    <row r="3" spans="1:30" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="21"/>
+    <row r="3" spans="1:30" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="43"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="3">
         <v>102</v>
       </c>
@@ -998,7 +1091,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="34">
-        <v>2.101</v>
+        <v>2101</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>7</v>
@@ -1028,9 +1121,9 @@
       <c r="AC3" s="10"/>
       <c r="AD3" s="10"/>
     </row>
-    <row r="4" spans="1:30" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="20" t="s">
+    <row r="4" spans="1:30" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="43"/>
+      <c r="B4" s="45" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="3">
@@ -1068,9 +1161,9 @@
       <c r="AC4" s="10"/>
       <c r="AD4" s="10"/>
     </row>
-    <row r="5" spans="1:30" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="23"/>
+    <row r="5" spans="1:30" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="43"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="3">
         <v>302</v>
       </c>
@@ -1083,9 +1176,9 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:30" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="23"/>
+    <row r="6" spans="1:30" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="43"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="3">
         <v>303</v>
       </c>
@@ -1093,7 +1186,7 @@
         <v>21</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>15</v>
@@ -1123,9 +1216,9 @@
       <c r="AC6" s="10"/>
       <c r="AD6" s="10"/>
     </row>
-    <row r="7" spans="1:30" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="23"/>
+    <row r="7" spans="1:30" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="43"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="3">
         <v>304</v>
       </c>
@@ -1161,9 +1254,9 @@
       <c r="AC7" s="10"/>
       <c r="AD7" s="10"/>
     </row>
-    <row r="8" spans="1:30" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="21"/>
+    <row r="8" spans="1:30" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="43"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="6">
         <v>305</v>
       </c>
@@ -1199,9 +1292,9 @@
       <c r="AC8" s="10"/>
       <c r="AD8" s="10"/>
     </row>
-    <row r="9" spans="1:30" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="22" t="s">
+    <row r="9" spans="1:30" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="43"/>
+      <c r="B9" s="48" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="18">
@@ -1210,8 +1303,8 @@
       <c r="D9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="35" t="s">
-        <v>32</v>
+      <c r="E9" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>15</v>
@@ -1241,9 +1334,9 @@
       <c r="AC9" s="10"/>
       <c r="AD9" s="10"/>
     </row>
-    <row r="10" spans="1:30" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="24"/>
+    <row r="10" spans="1:30" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="44"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="4">
         <v>402</v>
       </c>
@@ -1279,16 +1372,16 @@
       <c r="AC10" s="10"/>
       <c r="AD10" s="10"/>
     </row>
-    <row r="11" spans="1:30" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+    <row r="11" spans="1:30" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
       <c r="B11"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11"/>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+    <row r="12" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="23"/>
       <c r="B12"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
@@ -1319,7 +1412,7 @@
       <c r="AC12" s="10"/>
       <c r="AD12" s="10"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
     </row>
   </sheetData>
@@ -1334,25 +1427,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.5546875" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>33</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>24</v>
@@ -1373,173 +1467,282 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="25">
+        <v>101</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="26"/>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="51"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="25">
+        <v>102</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="36">
-        <v>101</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="37"/>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="36">
-        <v>102</v>
-      </c>
-      <c r="D3" s="36" t="s">
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="25">
+        <v>103</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="26"/>
+    </row>
+    <row r="5" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="51"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="25">
+        <v>104</v>
+      </c>
+      <c r="D5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="36">
-        <v>3.101</v>
-      </c>
-      <c r="F3" s="36" t="s">
+      <c r="E5" s="36">
+        <v>3101</v>
+      </c>
+      <c r="F5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="37"/>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="20" t="s">
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="51"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="25">
+        <v>105</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="36">
+        <v>3102</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="51"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="25">
+        <v>106</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="36">
+        <v>3103</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C8" s="25">
         <v>301</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D8" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36" t="s">
+      <c r="E8" s="25"/>
+      <c r="F8" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="37"/>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="36">
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="25">
         <v>302</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36" t="s">
+      <c r="D9" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="37"/>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="36">
+      <c r="G9" s="26"/>
+    </row>
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="25">
         <v>303</v>
       </c>
-      <c r="D6" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="36" t="s">
+      <c r="D10" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="37"/>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="36">
+      <c r="G10" s="26"/>
+    </row>
+    <row r="11" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="51"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="25">
         <v>304</v>
       </c>
-      <c r="D7" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36" t="s">
+      <c r="D11" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="37"/>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="38">
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="51"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="25">
         <v>305</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D12" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="51"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="25">
+        <v>306</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="27">
+        <v>307</v>
+      </c>
+      <c r="D14" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38" t="s">
+      <c r="E14" s="27"/>
+      <c r="F14" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="39"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="22" t="s">
+      <c r="G14" s="26"/>
+    </row>
+    <row r="15" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="51"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="27">
+        <v>308</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="28"/>
+    </row>
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="51"/>
+      <c r="B16" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C16" s="29">
         <v>401</v>
       </c>
-      <c r="D9" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="38" t="s">
+      <c r="D16" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="39"/>
-    </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="41">
+      <c r="G16" s="28"/>
+    </row>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="51"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="30">
         <v>402</v>
       </c>
-      <c r="D10" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41" t="s">
+      <c r="D17" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="42"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
+      <c r="G17" s="31"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="22"/>
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="21"/>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>